<commit_message>
update exampledata and diagrams
</commit_message>
<xml_diff>
--- a/sampledata/smartroom_exampledata.xlsx
+++ b/sampledata/smartroom_exampledata.xlsx
@@ -5,25 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\intellij\git\teaching.ws22.prse.smartroom.Team2\sampledata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2103B2B1-E190-4F4F-89B2-D448DBDF48FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CC4022-9B40-4F40-A8B3-C2DF090A6060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5890" yWindow="3390" windowWidth="24410" windowHeight="16900" tabRatio="736" xr2:uid="{28D1EC12-EB14-453E-A94E-4E36EE6F3C78}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="849" activeTab="2" xr2:uid="{28D1EC12-EB14-453E-A94E-4E36EE6F3C78}"/>
   </bookViews>
   <sheets>
     <sheet name="AirQualitySensorData" sheetId="10" r:id="rId1"/>
     <sheet name="AirQualitySensor" sheetId="11" r:id="rId2"/>
-    <sheet name="Room" sheetId="1" r:id="rId3"/>
-    <sheet name="Ventilator" sheetId="2" r:id="rId4"/>
-    <sheet name="Window" sheetId="3" r:id="rId5"/>
-    <sheet name="Door" sheetId="5" r:id="rId6"/>
-    <sheet name="Door_Connects_Room" sheetId="6" r:id="rId7"/>
-    <sheet name="PeopleInRoom" sheetId="8" r:id="rId8"/>
-    <sheet name="WindowOpen" sheetId="4" r:id="rId9"/>
-    <sheet name="DoorOpen" sheetId="7" r:id="rId10"/>
-    <sheet name="VentilatorOn" sheetId="9" r:id="rId11"/>
+    <sheet name="LightSource" sheetId="12" r:id="rId3"/>
+    <sheet name="LightSourceData" sheetId="13" r:id="rId4"/>
+    <sheet name="Room" sheetId="1" r:id="rId5"/>
+    <sheet name="Ventilator" sheetId="2" r:id="rId6"/>
+    <sheet name="Window" sheetId="3" r:id="rId7"/>
+    <sheet name="Door" sheetId="5" r:id="rId8"/>
+    <sheet name="Door_Connects_Room" sheetId="6" r:id="rId9"/>
+    <sheet name="PeopleInRoom" sheetId="8" r:id="rId10"/>
+    <sheet name="WindowOpen" sheetId="4" r:id="rId11"/>
+    <sheet name="DoorOpen" sheetId="7" r:id="rId12"/>
+    <sheet name="VentilatorOn" sheetId="9" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="72">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -169,9 +171,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>AirSensorID</t>
-  </si>
-  <si>
     <t>temperature</t>
   </si>
   <si>
@@ -257,6 +256,12 @@
   </si>
   <si>
     <t>0.44</t>
+  </si>
+  <si>
+    <t>LightSource_ID</t>
+  </si>
+  <si>
+    <t>AirQualitySensorID</t>
   </si>
 </sst>
 </file>
@@ -635,12 +640,12 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
@@ -651,16 +656,16 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -671,13 +676,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>250</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -688,13 +693,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>260</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -705,13 +710,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>270</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -722,13 +727,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>280</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -739,13 +744,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -756,13 +761,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>300</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -773,13 +778,13 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>310</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -790,13 +795,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>440</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -807,13 +812,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>470</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -824,13 +829,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>560</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -841,13 +846,13 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12">
         <v>600</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -858,13 +863,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>640</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -875,13 +880,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14">
         <v>680</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -892,13 +897,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>720</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -909,13 +914,13 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16">
         <v>760</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -926,13 +931,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17">
         <v>800</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -943,13 +948,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18">
         <v>840</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -960,13 +965,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19">
         <v>880</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -977,13 +982,13 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>920</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -993,6 +998,899 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480DF9BC-0BFB-4EE3-9B2B-FBC2D9C687DA}">
+  <dimension ref="A1:C58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2351F56-0462-4F03-B20B-D12C0A4A8EC7}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4ECEBBF-0275-445B-97B6-0AC89A61E978}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -1230,7 +2128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA42D3A5-CB57-44FD-8FC8-95D28FA40245}">
   <dimension ref="A1:C39"/>
   <sheetViews>
@@ -1687,6 +2585,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1718,6 +2619,290 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983CF047-4671-46AE-876C-F246F08894C3}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD9C3F7-E64B-481A-86F8-C14523F3382D}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FEFECF-7C26-4969-AB58-CF9427A50135}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1762,7 +2947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4491F75F-CCC3-4082-A162-5C98CE7F1123}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1799,7 +2984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49D6D91-1B8E-4513-A01B-7AA29E613961}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1860,7 +3045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2882436F-2B6C-4E07-BAC1-3E251526AFBC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -1897,7 +3082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE51B0-729E-4916-83B3-8669F753A99F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1948,897 +3133,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480DF9BC-0BFB-4EE3-9B2B-FBC2D9C687DA}">
-  <dimension ref="A1:C58"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2351F56-0462-4F03-B20B-D12C0A4A8EC7}">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>